<commit_message>
surasyti GPS modulio duomenys
</commit_message>
<xml_diff>
--- a/shieldu-pinai.xlsx
+++ b/shieldu-pinai.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\satur\Desktop\VSCode\f401_GPS_Shield\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF5A45BD-487F-4991-8CF2-9E2F0FF8FC79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="18210" yWindow="4635" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,9 +24,179 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>D15</t>
+  </si>
+  <si>
+    <t>D14</t>
+  </si>
+  <si>
+    <t>D13</t>
+  </si>
+  <si>
+    <t>D12</t>
+  </si>
+  <si>
+    <t>D11</t>
+  </si>
+  <si>
+    <t>D10</t>
+  </si>
+  <si>
+    <t>D9</t>
+  </si>
+  <si>
+    <t>D8</t>
+  </si>
+  <si>
+    <t>D7</t>
+  </si>
+  <si>
+    <t>D6</t>
+  </si>
+  <si>
+    <t>D5</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>B8</t>
+  </si>
+  <si>
+    <t>B9</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>A6</t>
+  </si>
+  <si>
+    <t>A7</t>
+  </si>
+  <si>
+    <t>B6</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>A9</t>
+  </si>
+  <si>
+    <t>A8</t>
+  </si>
+  <si>
+    <t>B10</t>
+  </si>
+  <si>
+    <t>B4</t>
+  </si>
+  <si>
+    <t>B5</t>
+  </si>
+  <si>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>A10</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>D0</t>
+  </si>
+  <si>
+    <t>GND</t>
+  </si>
+  <si>
+    <t>AVDD</t>
+  </si>
+  <si>
+    <t>GPS</t>
+  </si>
+  <si>
+    <t>WAKE_UP</t>
+  </si>
+  <si>
+    <t>I2C_SCL</t>
+  </si>
+  <si>
+    <t>I2C_SDA</t>
+  </si>
+  <si>
+    <t>Secondary</t>
+  </si>
+  <si>
+    <t>RESET</t>
+  </si>
+  <si>
+    <t>PPS</t>
+  </si>
+  <si>
+    <t>RX</t>
+  </si>
+  <si>
+    <t>TX</t>
+  </si>
+  <si>
+    <t>Jumper</t>
+  </si>
+  <si>
+    <t>J11</t>
+  </si>
+  <si>
+    <t>J12</t>
+  </si>
+  <si>
+    <t>J13</t>
+  </si>
+  <si>
+    <t>J10</t>
+  </si>
+  <si>
+    <t>J9</t>
+  </si>
+  <si>
+    <t>J7</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>J3</t>
+  </si>
+  <si>
+    <t>J4</t>
+  </si>
+  <si>
+    <t>J5</t>
+  </si>
+  <si>
+    <t>Default</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,16 +204,40 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -45,12 +245,164 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +682,309 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="E8:O28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M29" sqref="M29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="8" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="M8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+    </row>
+    <row r="9" spans="5:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M9" t="s">
+        <v>54</v>
+      </c>
+      <c r="N9" t="s">
+        <v>38</v>
+      </c>
+      <c r="O9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="K10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M10" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="N10" s="15"/>
+      <c r="O10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="K11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M11" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="N11" s="15"/>
+      <c r="O11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="K12" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="L12" s="17"/>
+    </row>
+    <row r="13" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="K13" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="L13" s="17"/>
+    </row>
+    <row r="14" spans="5:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="L14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="M14" t="s">
+        <v>35</v>
+      </c>
+      <c r="O14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E15" s="13"/>
+      <c r="F15" s="14">
+        <v>14</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="L15" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E16" s="9"/>
+      <c r="F16" s="10">
+        <v>13</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L16" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E17" s="9"/>
+      <c r="F17" s="10">
+        <v>12</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="L17" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E18" s="9"/>
+      <c r="F18" s="10">
+        <v>11</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="L18" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="N18" t="s">
+        <v>39</v>
+      </c>
+      <c r="O18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E19" s="9"/>
+      <c r="F19" s="10">
+        <v>10</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L19" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="N19" t="s">
+        <v>41</v>
+      </c>
+      <c r="O19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E20" s="9"/>
+      <c r="F20" s="10">
+        <v>9</v>
+      </c>
+      <c r="K20" s="16"/>
+      <c r="L20" s="17"/>
+    </row>
+    <row r="21" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E21" s="9"/>
+      <c r="F21" s="10">
+        <v>8</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L21" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M21" t="s">
+        <v>39</v>
+      </c>
+      <c r="O21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E22" s="9"/>
+      <c r="F22" s="10">
+        <v>7</v>
+      </c>
+      <c r="K22" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L22" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="M22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E23" s="9"/>
+      <c r="F23" s="10">
+        <v>6</v>
+      </c>
+      <c r="K23" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L23" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E24" s="9"/>
+      <c r="F24" s="10">
+        <v>5</v>
+      </c>
+      <c r="K24" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L24" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="N24" t="s">
+        <v>35</v>
+      </c>
+      <c r="O24" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E25" s="9"/>
+      <c r="F25" s="10">
+        <v>4</v>
+      </c>
+      <c r="K25" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L25" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E26" s="9"/>
+      <c r="F26" s="10">
+        <v>3</v>
+      </c>
+      <c r="K26" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L26" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M26" t="s">
+        <v>42</v>
+      </c>
+      <c r="O26" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E27" s="9"/>
+      <c r="F27" s="10">
+        <v>2</v>
+      </c>
+      <c r="K27" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="L27" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M27" t="s">
+        <v>41</v>
+      </c>
+      <c r="O27" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="5:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E28" s="11"/>
+      <c r="F28" s="12">
+        <v>1</v>
+      </c>
+      <c r="K28" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="L28" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="N28" t="s">
+        <v>42</v>
+      </c>
+      <c r="O28" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="M8:O8"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="K20:L20"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
surasyti sensoriaus pinai ir rastas jumperiu sprendimas
</commit_message>
<xml_diff>
--- a/shieldu-pinai.xlsx
+++ b/shieldu-pinai.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\satur\Desktop\VSCode\f401_GPS_Shield\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF5A45BD-487F-4991-8CF2-9E2F0FF8FC79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{544E913A-253A-4634-860D-C3BB2D69A314}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18210" yWindow="4635" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1785" yWindow="2205" windowWidth="21045" windowHeight="16245" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="72">
   <si>
     <t>D1</t>
   </si>
@@ -177,9 +177,6 @@
     <t>J7</t>
   </si>
   <si>
-    <t>J2</t>
-  </si>
-  <si>
     <t>J3</t>
   </si>
   <si>
@@ -190,6 +187,60 @@
   </si>
   <si>
     <t>Default</t>
+  </si>
+  <si>
+    <t>Sensoriai</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>A0</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>Veiksmas</t>
+  </si>
+  <si>
+    <t>LSM303AGR INT / DRDY</t>
+  </si>
+  <si>
+    <t>INT2 (DIL24)</t>
+  </si>
+  <si>
+    <t>LPS22HB INT1</t>
+  </si>
+  <si>
+    <t>LSM6DSL INT2</t>
+  </si>
+  <si>
+    <t>LSM6DSL INT1</t>
+  </si>
+  <si>
+    <t>USER INT</t>
+  </si>
+  <si>
+    <t>J6</t>
+  </si>
+  <si>
+    <t>SENS_J6 pakreipt sonu ant tu kur trumpinasi</t>
+  </si>
+  <si>
+    <t>JP11</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>J8 (PPS)</t>
+  </si>
+  <si>
+    <t>J6 -&gt; J8</t>
+  </si>
+  <si>
+    <t>J2-&gt;J3</t>
   </si>
 </sst>
 </file>
@@ -211,7 +262,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -236,8 +287,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -370,31 +427,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -403,6 +463,27 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -683,305 +764,469 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="E8:O28"/>
+  <dimension ref="A8:P28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M29" sqref="M29"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="11" max="11" width="9.7109375" customWidth="1"/>
+    <col min="14" max="14" width="9.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="8" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="M8" s="1" t="s">
+    <row r="8" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="J8" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
-    </row>
-    <row r="9" spans="5:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="M9" t="s">
+      <c r="K8" s="17"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="N9" t="s">
+      <c r="N8" s="17"/>
+      <c r="O8" s="17"/>
+      <c r="P8" s="19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="4:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J9" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="K9" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="O9" t="s">
+      <c r="L9" s="20" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="10" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="K10" s="2" t="s">
+      <c r="M9" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="N9" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="O9" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="P9" s="19"/>
+    </row>
+    <row r="10" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="H10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="L10" s="3" t="s">
+      <c r="I10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="M10" s="8" t="s">
+      <c r="J10" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="N10" s="15"/>
-      <c r="O10" t="s">
+      <c r="K10" s="13"/>
+      <c r="L10" s="22" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="11" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="K11" s="4" t="s">
+      <c r="M10" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="N10" s="13"/>
+      <c r="O10" s="20"/>
+      <c r="P10" s="19"/>
+    </row>
+    <row r="11" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="H11" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="L11" s="5" t="s">
+      <c r="I11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="M11" s="8" t="s">
+      <c r="J11" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="N11" s="15"/>
-      <c r="O11" t="s">
+      <c r="K11" s="13"/>
+      <c r="L11" s="22" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="12" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="K12" s="16" t="s">
+      <c r="M11" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="N11" s="13"/>
+      <c r="O11" s="20"/>
+      <c r="P11" s="19"/>
+    </row>
+    <row r="12" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="H12" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="L12" s="17"/>
-    </row>
-    <row r="13" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="K13" s="16" t="s">
+      <c r="I12" s="15"/>
+      <c r="M12" s="19"/>
+      <c r="N12" s="20"/>
+      <c r="O12" s="20"/>
+      <c r="P12" s="19"/>
+    </row>
+    <row r="13" spans="4:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H13" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="L13" s="17"/>
-    </row>
-    <row r="14" spans="5:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K14" s="4" t="s">
+      <c r="I13" s="15"/>
+      <c r="M13" s="19"/>
+      <c r="N13" s="20"/>
+      <c r="O13" s="20"/>
+      <c r="P13" s="19"/>
+    </row>
+    <row r="14" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D14" s="11"/>
+      <c r="E14" s="12">
+        <v>1</v>
+      </c>
+      <c r="H14" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="L14" s="5" t="s">
+      <c r="I14" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="M14" t="s">
+      <c r="J14" t="s">
         <v>35</v>
       </c>
-      <c r="O14" t="s">
+      <c r="L14" s="22" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="15" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E15" s="13"/>
-      <c r="F15" s="14">
+      <c r="M14" s="19"/>
+      <c r="N14" s="20"/>
+      <c r="O14" s="20"/>
+      <c r="P14" s="19"/>
+    </row>
+    <row r="15" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D15" s="7"/>
+      <c r="E15" s="8">
+        <v>2</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M15" s="19"/>
+      <c r="N15" s="20"/>
+      <c r="O15" s="20"/>
+      <c r="P15" s="19"/>
+    </row>
+    <row r="16" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D16" s="7"/>
+      <c r="E16" s="8">
+        <v>3</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M16" s="19"/>
+      <c r="N16" s="20"/>
+      <c r="O16" s="20"/>
+      <c r="P16" s="19"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D17" s="7"/>
+      <c r="E17" s="8">
+        <v>4</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="M17" s="19"/>
+      <c r="N17" s="20"/>
+      <c r="O17" s="20"/>
+      <c r="P17" s="19"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D18" s="7"/>
+      <c r="E18" s="8">
+        <v>5</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K18" t="s">
+        <v>39</v>
+      </c>
+      <c r="L18" t="s">
+        <v>47</v>
+      </c>
+      <c r="M18" s="19"/>
+      <c r="N18" s="20"/>
+      <c r="O18" s="20"/>
+      <c r="P18" s="19"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D19" s="7"/>
+      <c r="E19" s="8">
+        <v>6</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K19" t="s">
+        <v>41</v>
+      </c>
+      <c r="L19" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="M19" s="19"/>
+      <c r="N19" s="20"/>
+      <c r="O19" s="20"/>
+      <c r="P19" s="19"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D20" s="7"/>
+      <c r="E20" s="8">
+        <v>7</v>
+      </c>
+      <c r="H20" s="14"/>
+      <c r="I20" s="15"/>
+      <c r="M20" s="19"/>
+      <c r="N20" s="20"/>
+      <c r="O20" s="20"/>
+      <c r="P20" s="19"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D21" s="7"/>
+      <c r="E21" s="8">
+        <v>8</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J21" t="s">
+        <v>39</v>
+      </c>
+      <c r="L21" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="M21" s="19"/>
+      <c r="N21" s="20"/>
+      <c r="O21" s="20"/>
+      <c r="P21" s="19"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D22" s="7"/>
+      <c r="E22" s="8"/>
+      <c r="H22" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J22" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="L22" t="s">
+        <v>65</v>
+      </c>
+      <c r="M22" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="N22" s="20"/>
+      <c r="O22" s="20"/>
+      <c r="P22" s="19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D23" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E23" s="8">
+        <v>1</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="M23" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="N23" s="20"/>
+      <c r="O23" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="P23" s="19"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D24" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E24" s="8">
+        <v>2</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K24" t="s">
+        <v>35</v>
+      </c>
+      <c r="L24" t="s">
+        <v>49</v>
+      </c>
+      <c r="M24" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="N24" s="20"/>
+      <c r="O24" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="P24" s="19"/>
+    </row>
+    <row r="25" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" s="13"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E25" s="8">
+        <v>3</v>
+      </c>
+      <c r="H25" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="K15" s="4" t="s">
+      <c r="I25" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="M25" s="19"/>
+      <c r="N25" s="20"/>
+      <c r="O25" s="20"/>
+      <c r="P25" s="19"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" s="13"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E26" s="8">
+        <v>4</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J26" t="s">
+        <v>42</v>
+      </c>
+      <c r="L26" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="M26" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="N26" s="20"/>
+      <c r="O26" s="20"/>
+      <c r="P26" s="19" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A27" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" s="23"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E27" s="8">
         <v>5</v>
       </c>
-      <c r="L15" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E16" s="9"/>
-      <c r="F16" s="10">
-        <v>13</v>
-      </c>
-      <c r="K16" s="4" t="s">
+      <c r="H27" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J27" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="K27" t="s">
+        <v>40</v>
+      </c>
+      <c r="L27" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="M27" s="19"/>
+      <c r="N27" s="20"/>
+      <c r="O27" s="20"/>
+      <c r="P27" s="19" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="23"/>
+      <c r="B28" s="23"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E28" s="10">
         <v>6</v>
       </c>
-      <c r="L16" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E17" s="9"/>
-      <c r="F17" s="10">
-        <v>12</v>
-      </c>
-      <c r="K17" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="L17" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E18" s="9"/>
-      <c r="F18" s="10">
-        <v>11</v>
-      </c>
-      <c r="K18" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="L18" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="N18" t="s">
-        <v>39</v>
-      </c>
-      <c r="O18" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E19" s="9"/>
-      <c r="F19" s="10">
-        <v>10</v>
-      </c>
-      <c r="K19" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="L19" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="N19" t="s">
-        <v>41</v>
-      </c>
-      <c r="O19" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="20" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E20" s="9"/>
-      <c r="F20" s="10">
-        <v>9</v>
-      </c>
-      <c r="K20" s="16"/>
-      <c r="L20" s="17"/>
-    </row>
-    <row r="21" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E21" s="9"/>
-      <c r="F21" s="10">
-        <v>8</v>
-      </c>
-      <c r="K21" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="L21" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="M21" t="s">
-        <v>39</v>
-      </c>
-      <c r="O21" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E22" s="9"/>
-      <c r="F22" s="10">
-        <v>7</v>
-      </c>
-      <c r="K22" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="L22" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="M22" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E23" s="9"/>
-      <c r="F23" s="10">
-        <v>6</v>
-      </c>
-      <c r="K23" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="L23" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E24" s="9"/>
-      <c r="F24" s="10">
-        <v>5</v>
-      </c>
-      <c r="K24" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="L24" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="N24" t="s">
-        <v>35</v>
-      </c>
-      <c r="O24" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="25" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E25" s="9"/>
-      <c r="F25" s="10">
-        <v>4</v>
-      </c>
-      <c r="K25" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L25" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="26" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E26" s="9"/>
-      <c r="F26" s="10">
-        <v>3</v>
-      </c>
-      <c r="K26" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="L26" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="M26" t="s">
+      <c r="H28" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I28" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K28" t="s">
         <v>42</v>
       </c>
-      <c r="O26" t="s">
+      <c r="L28" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="27" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E27" s="9"/>
-      <c r="F27" s="10">
-        <v>2</v>
-      </c>
-      <c r="K27" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="L27" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="M27" t="s">
-        <v>41</v>
-      </c>
-      <c r="O27" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="28" spans="5:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E28" s="11"/>
-      <c r="F28" s="12">
-        <v>1</v>
-      </c>
-      <c r="K28" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="L28" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="N28" t="s">
-        <v>42</v>
-      </c>
-      <c r="O28" t="s">
-        <v>53</v>
-      </c>
+      <c r="M28" s="19"/>
+      <c r="N28" s="20"/>
+      <c r="O28" s="20"/>
+      <c r="P28" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="12">
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A27:C28"/>
+    <mergeCell ref="H20:I20"/>
     <mergeCell ref="M8:O8"/>
     <mergeCell ref="M10:N10"/>
     <mergeCell ref="M11:N11"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H13:I13"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>